<commit_message>
Updating weather data + readme
</commit_message>
<xml_diff>
--- a/data/BostonMarathonWeather-00-24.xlsx
+++ b/data/BostonMarathonWeather-00-24.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dell-my.sharepoint.com/personal/calvin_cuff_dell_com/Documents/Documents/Grad School/DACSS 603/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuffc3\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C3D49AC-8110-4D08-8979-A881A3849CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CB63DE-EC04-48E7-B574-DDB5C9962F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="12495" windowWidth="29040" windowHeight="15720" xr2:uid="{EE6896E5-5B19-4D19-BED7-90ACBEEFB9A8}"/>
+    <workbookView xWindow="86280" yWindow="10770" windowWidth="29040" windowHeight="15720" xr2:uid="{EE6896E5-5B19-4D19-BED7-90ACBEEFB9A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>RaceYear</t>
   </si>
@@ -133,6 +132,30 @@
   </si>
   <si>
     <t>https://www.boston-discovery-guide.com/boston-marathon-weather.html</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Rainfall (in)</t>
+  </si>
+  <si>
+    <t>https://www.wunderground.com/history/daily/us/ma/east-boston/KBOS/date/2006-4-17</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>Max_WindSPeed</t>
+  </si>
+  <si>
+    <t>Dew Point_avg</t>
+  </si>
+  <si>
+    <t>Dew_point_Hi</t>
+  </si>
+  <si>
+    <t>Dew_point_low</t>
   </si>
 </sst>
 </file>
@@ -177,9 +200,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,682 +519,1219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC096DC8-8A9B-4B60-95D6-2440D88AE290}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="6" max="6" width="11.26171875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="8.83984375" customWidth="1"/>
+    <col min="9" max="9" width="12.578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.578125" customWidth="1"/>
+    <col min="11" max="11" width="13.1015625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.26171875" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="8.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
+      <c r="O1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2">
+        <v>45397</v>
+      </c>
+      <c r="B2">
         <v>2024</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>67</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>46</v>
       </c>
-      <c r="D2">
+      <c r="E2">
+        <v>58</v>
+      </c>
+      <c r="F2">
+        <v>23</v>
+      </c>
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="I2">
+        <v>48</v>
+      </c>
+      <c r="J2">
+        <v>33</v>
+      </c>
+      <c r="K2">
+        <v>42.68</v>
+      </c>
+      <c r="L2">
         <v>0.72</v>
       </c>
-      <c r="G2" t="s">
+      <c r="M2" t="s">
         <v>11</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2">
+        <v>45033</v>
+      </c>
+      <c r="B3">
         <v>2023</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>56</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>47</v>
       </c>
-      <c r="D3">
+      <c r="E3">
+        <v>48.77</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="F3">
+      <c r="I3">
+        <v>51</v>
+      </c>
+      <c r="J3">
+        <v>46</v>
+      </c>
+      <c r="K3">
+        <v>48.52</v>
+      </c>
+      <c r="L3">
         <v>0.99</v>
       </c>
-      <c r="G3" t="s">
+      <c r="M3" t="s">
         <v>13</v>
       </c>
-      <c r="H3">
+      <c r="N3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
+      <c r="O3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2">
+        <v>44669</v>
+      </c>
+      <c r="B4">
         <v>2022</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>54</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>37</v>
       </c>
-      <c r="D4">
+      <c r="E4">
+        <v>45.24</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="F4">
+      <c r="I4">
+        <v>39</v>
+      </c>
+      <c r="J4">
+        <v>24</v>
+      </c>
+      <c r="K4">
+        <v>31.32</v>
+      </c>
+      <c r="L4">
         <v>0.43</v>
       </c>
-      <c r="G4" t="s">
+      <c r="M4" t="s">
         <v>14</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2">
+        <v>44480</v>
+      </c>
+      <c r="B5">
         <v>2021</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>69</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>62</v>
       </c>
-      <c r="D5">
+      <c r="E5">
+        <v>64.239999999999995</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>7</v>
       </c>
-      <c r="F5">
+      <c r="I5">
+        <v>60</v>
+      </c>
+      <c r="J5">
+        <v>57</v>
+      </c>
+      <c r="K5">
+        <v>58.88</v>
+      </c>
+      <c r="L5">
         <v>0.88</v>
       </c>
-      <c r="G5" t="s">
+      <c r="M5" t="s">
         <v>15</v>
       </c>
-      <c r="H5">
+      <c r="N5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2">
+        <v>43570</v>
+      </c>
+      <c r="B6">
         <v>2019</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>68</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>46</v>
       </c>
-      <c r="D6">
+      <c r="E6">
+        <v>55.82</v>
+      </c>
+      <c r="F6">
+        <v>26</v>
+      </c>
+      <c r="G6">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>16</v>
       </c>
-      <c r="F6">
+      <c r="I6">
+        <v>62</v>
+      </c>
+      <c r="J6">
+        <v>28</v>
+      </c>
+      <c r="K6">
+        <v>49.26</v>
+      </c>
+      <c r="L6">
         <v>0.87</v>
       </c>
-      <c r="G6" t="s">
+      <c r="M6" t="s">
         <v>13</v>
       </c>
-      <c r="H6">
+      <c r="N6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
+      <c r="O6">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2">
+        <v>43206</v>
+      </c>
+      <c r="B7">
         <v>2018</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>50</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>35</v>
       </c>
-      <c r="D7">
+      <c r="E7">
+        <v>43.18</v>
+      </c>
+      <c r="F7">
+        <v>31</v>
+      </c>
+      <c r="G7">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>7</v>
       </c>
-      <c r="F7">
+      <c r="I7">
+        <v>52</v>
+      </c>
+      <c r="J7">
+        <v>33</v>
+      </c>
+      <c r="K7">
+        <v>42.32</v>
+      </c>
+      <c r="L7">
         <v>0.89</v>
       </c>
-      <c r="G7" t="s">
+      <c r="M7" t="s">
         <v>8</v>
       </c>
-      <c r="H7">
+      <c r="N7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
+      <c r="O7">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2">
+        <v>42842</v>
+      </c>
+      <c r="B8">
         <v>2017</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>71</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>42</v>
       </c>
-      <c r="D8">
+      <c r="E8">
+        <v>65.87</v>
+      </c>
+      <c r="F8">
+        <v>22</v>
+      </c>
+      <c r="G8">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>17</v>
       </c>
-      <c r="F8">
+      <c r="I8">
+        <v>57</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>43.09</v>
+      </c>
+      <c r="L8">
         <v>0.37</v>
       </c>
-      <c r="G8" t="s">
+      <c r="M8" t="s">
         <v>18</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2">
+        <v>42478</v>
+      </c>
+      <c r="B9">
         <v>2016</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>71</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>48</v>
       </c>
-      <c r="D9">
+      <c r="E9">
+        <v>50.96</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>12</v>
       </c>
-      <c r="F9">
+      <c r="I9">
+        <v>37</v>
+      </c>
+      <c r="J9">
+        <v>30</v>
+      </c>
+      <c r="K9">
+        <v>34.21</v>
+      </c>
+      <c r="L9">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G9" t="s">
+      <c r="M9" t="s">
         <v>19</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2">
+        <v>42114</v>
+      </c>
+      <c r="B10">
         <v>2015</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>44</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>40</v>
       </c>
-      <c r="D10">
+      <c r="E10">
+        <v>44.74</v>
+      </c>
+      <c r="F10">
+        <v>22</v>
+      </c>
+      <c r="G10">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>20</v>
       </c>
-      <c r="F10">
+      <c r="I10">
+        <v>51</v>
+      </c>
+      <c r="J10">
+        <v>35</v>
+      </c>
+      <c r="K10">
+        <v>42.4</v>
+      </c>
+      <c r="L10">
         <v>0.93</v>
       </c>
-      <c r="G10" t="s">
+      <c r="M10" t="s">
         <v>21</v>
       </c>
-      <c r="H10">
+      <c r="N10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
+      <c r="O10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2">
+        <v>41750</v>
+      </c>
+      <c r="B11">
         <v>2014</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>63</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>36</v>
       </c>
-      <c r="D11">
+      <c r="E11">
+        <v>51.38</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
+      <c r="H11" t="s">
         <v>22</v>
       </c>
-      <c r="F11">
+      <c r="I11">
+        <v>38</v>
+      </c>
+      <c r="J11">
+        <v>23</v>
+      </c>
+      <c r="K11">
+        <v>32.21</v>
+      </c>
+      <c r="L11">
         <v>0.24</v>
       </c>
-      <c r="G11" t="s">
+      <c r="M11" t="s">
         <v>18</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2">
+        <v>41379</v>
+      </c>
+      <c r="B12">
         <v>2013</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>55</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>37</v>
       </c>
-      <c r="D12">
+      <c r="E12">
+        <v>44.83</v>
+      </c>
+      <c r="F12">
+        <v>18</v>
+      </c>
+      <c r="G12">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
+      <c r="H12" t="s">
         <v>7</v>
       </c>
-      <c r="F12">
+      <c r="I12">
+        <v>29.78</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>29.78</v>
+      </c>
+      <c r="L12">
         <v>0.48</v>
       </c>
-      <c r="G12" t="s">
+      <c r="M12" t="s">
         <v>23</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2">
+        <v>41015</v>
+      </c>
+      <c r="B13">
         <v>2012</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>91</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>54</v>
       </c>
-      <c r="D13">
+      <c r="E13">
+        <v>71.09</v>
+      </c>
+      <c r="F13">
+        <v>18</v>
+      </c>
+      <c r="G13">
         <v>9</v>
       </c>
-      <c r="E13" t="s">
+      <c r="H13" t="s">
         <v>24</v>
       </c>
-      <c r="F13">
+      <c r="I13">
+        <v>58</v>
+      </c>
+      <c r="J13">
+        <v>52</v>
+      </c>
+      <c r="K13">
+        <v>55.43</v>
+      </c>
+      <c r="L13">
         <v>0.46</v>
       </c>
-      <c r="G13" t="s">
+      <c r="M13" t="s">
         <v>18</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14">
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2">
+        <v>40651</v>
+      </c>
+      <c r="B14">
         <v>2011</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>64</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>44</v>
       </c>
-      <c r="D14">
+      <c r="E14">
+        <v>52.58</v>
+      </c>
+      <c r="F14">
+        <v>25</v>
+      </c>
+      <c r="G14">
         <v>20</v>
       </c>
-      <c r="E14" t="s">
+      <c r="H14" t="s">
         <v>3</v>
       </c>
-      <c r="F14">
+      <c r="I14">
+        <v>37</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>27.67</v>
+      </c>
+      <c r="L14">
         <v>0.43</v>
       </c>
-      <c r="G14" t="s">
+      <c r="M14" t="s">
         <v>15</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="2">
+        <v>40287</v>
+      </c>
+      <c r="B15">
         <v>2010</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>60</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>34</v>
       </c>
-      <c r="D15">
+      <c r="E15">
+        <v>50.39</v>
+      </c>
+      <c r="F15">
+        <v>18</v>
+      </c>
+      <c r="G15">
         <v>12</v>
       </c>
-      <c r="E15" t="s">
+      <c r="H15" t="s">
         <v>25</v>
       </c>
-      <c r="F15">
+      <c r="I15">
+        <v>37</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>31.78</v>
+      </c>
+      <c r="L15">
         <v>0.5</v>
       </c>
-      <c r="G15" t="s">
+      <c r="M15" t="s">
         <v>15</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16">
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="2">
+        <v>39923</v>
+      </c>
+      <c r="B16">
         <v>2009</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>53</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>28</v>
       </c>
-      <c r="D16">
+      <c r="E16">
+        <v>43.56</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16">
         <v>9</v>
       </c>
-      <c r="E16" t="s">
+      <c r="H16" t="s">
         <v>9</v>
       </c>
-      <c r="F16">
+      <c r="I16">
+        <v>40</v>
+      </c>
+      <c r="J16">
+        <v>35</v>
+      </c>
+      <c r="K16">
+        <v>37.880000000000003</v>
+      </c>
+      <c r="L16">
         <v>0.7</v>
       </c>
-      <c r="G16" t="s">
+      <c r="M16" t="s">
         <v>18</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17">
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="2">
+        <v>39559</v>
+      </c>
+      <c r="B17">
         <v>2008</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>64</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>42</v>
       </c>
-      <c r="D17">
+      <c r="E17">
+        <v>47.85</v>
+      </c>
+      <c r="F17">
+        <v>13</v>
+      </c>
+      <c r="G17">
         <v>3</v>
       </c>
-      <c r="E17" t="s">
+      <c r="H17" t="s">
         <v>20</v>
       </c>
-      <c r="F17">
+      <c r="I17">
+        <v>44</v>
+      </c>
+      <c r="J17">
+        <v>41</v>
+      </c>
+      <c r="K17">
+        <v>42.74</v>
+      </c>
+      <c r="L17">
         <v>0.83</v>
       </c>
-      <c r="G17" t="s">
+      <c r="M17" t="s">
         <v>13</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="2">
+        <v>39188</v>
+      </c>
+      <c r="B18">
         <v>2007</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>51</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>38</v>
       </c>
-      <c r="D18">
+      <c r="E18">
+        <v>45.6</v>
+      </c>
+      <c r="F18">
+        <v>39</v>
+      </c>
+      <c r="G18">
         <v>14</v>
       </c>
-      <c r="E18" t="s">
+      <c r="H18" t="s">
         <v>9</v>
       </c>
-      <c r="F18">
+      <c r="I18">
+        <v>47</v>
+      </c>
+      <c r="J18">
+        <v>38</v>
+      </c>
+      <c r="K18">
+        <v>43.09</v>
+      </c>
+      <c r="L18">
         <v>0.87</v>
       </c>
-      <c r="G18" t="s">
+      <c r="M18" t="s">
         <v>13</v>
       </c>
-      <c r="H18">
+      <c r="N18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
+      <c r="O18">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="2">
+        <v>38824</v>
+      </c>
+      <c r="B19">
         <v>2006</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>61</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>33</v>
       </c>
-      <c r="D19">
+      <c r="E19">
+        <v>47.44</v>
+      </c>
+      <c r="F19">
+        <v>16</v>
+      </c>
+      <c r="G19">
         <v>8</v>
       </c>
-      <c r="E19" t="s">
+      <c r="H19" t="s">
         <v>26</v>
       </c>
-      <c r="F19">
+      <c r="I19">
+        <v>38</v>
+      </c>
+      <c r="J19">
+        <v>33</v>
+      </c>
+      <c r="K19">
+        <v>35.24</v>
+      </c>
+      <c r="L19">
         <v>0.5</v>
       </c>
-      <c r="G19" t="s">
+      <c r="M19" t="s">
         <v>13</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="2">
+        <v>38460</v>
+      </c>
+      <c r="B20">
         <v>2005</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>73</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>37</v>
       </c>
-      <c r="D20">
+      <c r="E20">
+        <v>56.42</v>
+      </c>
+      <c r="F20">
+        <v>15</v>
+      </c>
+      <c r="G20">
         <v>6</v>
       </c>
-      <c r="E20" t="s">
+      <c r="H20" t="s">
         <v>27</v>
       </c>
-      <c r="F20">
+      <c r="I20">
+        <v>33</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>25.54</v>
+      </c>
+      <c r="L20">
         <v>0.11</v>
       </c>
-      <c r="G20" t="s">
+      <c r="M20" t="s">
         <v>15</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="2">
+        <v>38096</v>
+      </c>
+      <c r="B21">
         <v>2004</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>84</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>46</v>
       </c>
-      <c r="D21">
+      <c r="E21">
+        <v>62.54</v>
+      </c>
+      <c r="F21">
+        <v>29</v>
+      </c>
+      <c r="G21">
         <v>18</v>
       </c>
-      <c r="E21" t="s">
+      <c r="H21" t="s">
         <v>24</v>
       </c>
-      <c r="F21">
+      <c r="I21">
+        <v>51</v>
+      </c>
+      <c r="J21">
+        <v>40</v>
+      </c>
+      <c r="K21">
+        <v>46.15</v>
+      </c>
+      <c r="L21">
         <v>0.32</v>
       </c>
-      <c r="G21" t="s">
+      <c r="M21" t="s">
         <v>18</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22">
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="2">
+        <v>37732</v>
+      </c>
+      <c r="B22">
         <v>2003</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>69</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>32</v>
       </c>
-      <c r="D22">
+      <c r="E22">
+        <v>47.3</v>
+      </c>
+      <c r="F22">
+        <v>25</v>
+      </c>
+      <c r="G22">
         <v>10</v>
       </c>
-      <c r="E22" t="s">
+      <c r="H22" t="s">
         <v>28</v>
       </c>
-      <c r="F22">
+      <c r="I22">
+        <v>42</v>
+      </c>
+      <c r="J22">
+        <v>35</v>
+      </c>
+      <c r="K22">
+        <v>37.74</v>
+      </c>
+      <c r="L22">
         <v>0.35</v>
       </c>
-      <c r="G22" t="s">
+      <c r="M22" t="s">
         <v>18</v>
       </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23">
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="2">
+        <v>37361</v>
+      </c>
+      <c r="B23">
         <v>2002</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>66</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>46</v>
       </c>
-      <c r="D23">
+      <c r="E23">
+        <v>49.64</v>
+      </c>
+      <c r="F23">
+        <v>15</v>
+      </c>
+      <c r="G23">
         <v>6</v>
       </c>
-      <c r="E23" t="s">
+      <c r="H23" t="s">
         <v>27</v>
       </c>
-      <c r="F23">
+      <c r="I23">
+        <v>56</v>
+      </c>
+      <c r="J23">
+        <v>45</v>
+      </c>
+      <c r="K23">
+        <v>48.22</v>
+      </c>
+      <c r="L23">
         <v>1</v>
       </c>
-      <c r="G23" t="s">
+      <c r="M23" t="s">
         <v>29</v>
       </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24">
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="2">
+        <v>36997</v>
+      </c>
+      <c r="B24">
         <v>2001</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>57</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>35</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="E24">
+        <v>43.83</v>
+      </c>
+      <c r="F24">
+        <v>15</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
         <v>7</v>
       </c>
-      <c r="F24">
+      <c r="I24">
+        <v>41</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>33.78</v>
+      </c>
+      <c r="L24">
         <v>0.32</v>
       </c>
-      <c r="G24" t="s">
+      <c r="M24" t="s">
         <v>18</v>
       </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25">
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="2">
+        <v>36633</v>
+      </c>
+      <c r="B25">
         <v>2000</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>48</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>39</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="E25">
+        <v>43</v>
+      </c>
+      <c r="F25">
+        <v>21</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
         <v>12</v>
       </c>
-      <c r="F25">
+      <c r="I25">
+        <v>39</v>
+      </c>
+      <c r="J25">
+        <v>27</v>
+      </c>
+      <c r="K25">
+        <v>30.43</v>
+      </c>
+      <c r="L25">
         <v>0.47</v>
       </c>
-      <c r="G25" t="s">
+      <c r="M25" t="s">
         <v>13</v>
       </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="1" t="s">
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="D28" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C29" t="s">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="D29" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="D30" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C28" r:id="rId1" xr:uid="{58389F77-6A69-426A-93D4-9D50720E3A5B}"/>
+    <hyperlink ref="D28" r:id="rId1" xr:uid="{58389F77-6A69-426A-93D4-9D50720E3A5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>